<commit_message>
updated digikey links for BQ24075 and BGM13P
</commit_message>
<xml_diff>
--- a/Gateway/Project Outputs for Gateway/Gateway.xlsx
+++ b/Gateway/Project Outputs for Gateway/Gateway.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2DC1308-F3DE-46EB-B648-39CE088494AE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CDFB0248-E50D-410E-8DFF-6D3B1AE7ABD5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13110" windowHeight="7995" xr2:uid="{26608945-8CB5-47E7-A5DA-667274689EFB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13110" windowHeight="7995" xr2:uid="{F8D59719-2269-440C-ABEA-8661FA29D0C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Gateway" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="143">
   <si>
     <t>Description</t>
   </si>
@@ -37,6 +37,123 @@
     <t>Quantity</t>
   </si>
   <si>
+    <t>Header, 10-Pin</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Header, 2-Pin</t>
+  </si>
+  <si>
+    <t>P2, P3</t>
+  </si>
+  <si>
+    <t>PC TEST POINT MINIATURE</t>
+  </si>
+  <si>
+    <t>TP1, TP2, TP3, TP5, TP6, TP10, TP11</t>
+  </si>
+  <si>
+    <t>36-5019CT-ND</t>
+  </si>
+  <si>
+    <t>5019</t>
+  </si>
+  <si>
+    <t>TVS DIODE 5.5V 14V 2X1SON</t>
+  </si>
+  <si>
+    <t>D18, D19, D20, D21, D22</t>
+  </si>
+  <si>
+    <t>296-30406-1-ND</t>
+  </si>
+  <si>
+    <t>TPD1E10B06DPYR</t>
+  </si>
+  <si>
+    <t>Zener Diode</t>
+  </si>
+  <si>
+    <t>D4, D8, D9, D10, D11, D12, D13, D14, D15, D16, D17, D25, D26, D27, D28, D29</t>
+  </si>
+  <si>
+    <t>IC LI-ION CHARGE MGMT 16-QFN</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>296-38874-1-ND</t>
+  </si>
+  <si>
+    <t>BQ24075RGTR</t>
+  </si>
+  <si>
+    <t>Tiny Single Inductor Buck Boost Converter 12-VQFN -40 to 85</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>296-42650-1-ND</t>
+  </si>
+  <si>
+    <t>TPS63051RMWR</t>
+  </si>
+  <si>
+    <t>EFR32BG13 Bluetooth 5.0 Module, 512kB Flash, +8dbm</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>336-5465-1-ND</t>
+  </si>
+  <si>
+    <t>BGM13P22F512GA-V2</t>
+  </si>
+  <si>
+    <t>CAP CER 1300PF 25V C0G/NP0 0603</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>399-14953-1-ND</t>
+  </si>
+  <si>
+    <t>C0603C132J3GAC7867</t>
+  </si>
+  <si>
+    <t>SWITCH SLIDE SPDT 100MA 12V</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>401-2012-1-ND</t>
+  </si>
+  <si>
+    <t>AYZ0102AGRLC</t>
+  </si>
+  <si>
+    <t>MHS22204=DPDT SL SW VERT AG</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>450-1572-ND</t>
+  </si>
+  <si>
+    <t>1825289-1</t>
+  </si>
+  <si>
     <t>CONN HEADER PH SIDE 2POS 2MM SMD</t>
   </si>
   <si>
@@ -49,6 +166,87 @@
     <t>S2B-PH-SM4-TB(LF)(SN)</t>
   </si>
   <si>
+    <t>LED RED DIFFUSED 0603 SMD</t>
+  </si>
+  <si>
+    <t>D23</t>
+  </si>
+  <si>
+    <t>475-1195-1-ND</t>
+  </si>
+  <si>
+    <t>LS L29K-H1J2-1-Z</t>
+  </si>
+  <si>
+    <t>LED YELLOW DIFFUSED 0603 SMD</t>
+  </si>
+  <si>
+    <t>D24</t>
+  </si>
+  <si>
+    <t>475-1196-1-ND</t>
+  </si>
+  <si>
+    <t>LY L29K-H1K2-26-Z</t>
+  </si>
+  <si>
+    <t>Blue 470nm LED Indication - Discrete 2.85V 0603 (1608 Metric)</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>475-2816-1-ND</t>
+  </si>
+  <si>
+    <t>LB Q39G-L2OO-35-1</t>
+  </si>
+  <si>
+    <t>LED GREEN DIFFUSED 0603 SMD</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>475-3118-1-ND</t>
+  </si>
+  <si>
+    <t>LG L29K-F2J1-24-Z</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>CAP CER 1000PF 50V X7R 0603</t>
+  </si>
+  <si>
+    <t>C9, C10</t>
+  </si>
+  <si>
+    <t>478-5006-1-ND</t>
+  </si>
+  <si>
+    <t>06035C102JAT2A</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 16V X7R 0603</t>
+  </si>
+  <si>
+    <t>C11, C12</t>
+  </si>
+  <si>
+    <t>478-7617-1-ND</t>
+  </si>
+  <si>
+    <t>0603YC104MAT4A</t>
+  </si>
+  <si>
     <t>CAP CER 0.1UF 25V X7R 0603</t>
   </si>
   <si>
@@ -73,117 +271,6 @@
     <t>GRM188R61A106KE69D</t>
   </si>
   <si>
-    <t>CAP CER 1300PF 25V C0G/NP0 0603</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>399-14953-1-ND</t>
-  </si>
-  <si>
-    <t>C0603C132J3GAC7867</t>
-  </si>
-  <si>
-    <t>CAP CER 1000PF 50V X7R 0603</t>
-  </si>
-  <si>
-    <t>C9, C10</t>
-  </si>
-  <si>
-    <t>478-5006-1-ND</t>
-  </si>
-  <si>
-    <t>06035C102JAT2A</t>
-  </si>
-  <si>
-    <t>CAP CER 0.1UF 16V X7R 0603</t>
-  </si>
-  <si>
-    <t>C11, C12</t>
-  </si>
-  <si>
-    <t>478-7617-1-ND</t>
-  </si>
-  <si>
-    <t>0603YC104MAT4A</t>
-  </si>
-  <si>
-    <t>Blue 470nm LED Indication - Discrete 2.85V 0603 (1608 Metric)</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>475-2816-1-ND</t>
-  </si>
-  <si>
-    <t>LB Q39G-L2OO-35-1</t>
-  </si>
-  <si>
-    <t>LED GREEN DIFFUSED 0603 SMD</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>475-3118-1-ND</t>
-  </si>
-  <si>
-    <t>LG L29K-F2J1-24-Z</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>Zener Diode</t>
-  </si>
-  <si>
-    <t>D4, D8, D9, D10, D11, D12, D13, D14, D15, D16, D17, D25, D26, D27, D28, D29</t>
-  </si>
-  <si>
-    <t>296-30406-1-ND</t>
-  </si>
-  <si>
-    <t>TPD1E10B06DPYR</t>
-  </si>
-  <si>
-    <t>D6</t>
-  </si>
-  <si>
-    <t>D7</t>
-  </si>
-  <si>
-    <t>TVS DIODE 5.5V 14V 2X1SON</t>
-  </si>
-  <si>
-    <t>D18, D19, D20, D21, D22</t>
-  </si>
-  <si>
-    <t>LED RED DIFFUSED 0603 SMD</t>
-  </si>
-  <si>
-    <t>D23</t>
-  </si>
-  <si>
-    <t>475-1195-1-ND</t>
-  </si>
-  <si>
-    <t>LS L29K-H1J2-1-Z</t>
-  </si>
-  <si>
-    <t>LED YELLOW DIFFUSED 0603 SMD</t>
-  </si>
-  <si>
-    <t>D24</t>
-  </si>
-  <si>
-    <t>475-1196-1-ND</t>
-  </si>
-  <si>
-    <t>LY L29K-H1K2-26-Z</t>
-  </si>
-  <si>
     <t>FIXED IND 1.5UH 1.1A 213 MOHM</t>
   </si>
   <si>
@@ -196,6 +283,18 @@
     <t>LQM18PN1R5MFHD</t>
   </si>
   <si>
+    <t>RES SMD 100 OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R18, R19, R22</t>
+  </si>
+  <si>
+    <t>541-4059-1-ND</t>
+  </si>
+  <si>
+    <t>CRCW0603100RJNEAC</t>
+  </si>
+  <si>
     <t>Micro Usb, 2.0 Type Ab, Receptacle, Th</t>
   </si>
   <si>
@@ -208,13 +307,124 @@
     <t>10104111-0001LF</t>
   </si>
   <si>
-    <t>Header, 2-Pin</t>
-  </si>
-  <si>
-    <t>P2, P3</t>
-  </si>
-  <si>
-    <t/>
+    <t>SWITCH TACTILE SPST-NO 0.05A 12V</t>
+  </si>
+  <si>
+    <t>S3, S4, S5</t>
+  </si>
+  <si>
+    <t>732-7004-1-ND</t>
+  </si>
+  <si>
+    <t>430182043816</t>
+  </si>
+  <si>
+    <t>RES 0 OHM JUMPER 1/8W 0603</t>
+  </si>
+  <si>
+    <t>R3, R11, R25</t>
+  </si>
+  <si>
+    <t>749-1745-1-ND</t>
+  </si>
+  <si>
+    <t>MCT0603MZ0000ZP500</t>
+  </si>
+  <si>
+    <t>USB Bridge, USB to UART USB 2.0 UART Interface 28-SSOP</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>768-1007-1-ND</t>
+  </si>
+  <si>
+    <t>FT232RL-REEL</t>
+  </si>
+  <si>
+    <t>RES SMD 1M OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R16, R17</t>
+  </si>
+  <si>
+    <t>1276-5134-1-ND</t>
+  </si>
+  <si>
+    <t>RC1608J105CS</t>
+  </si>
+  <si>
+    <t>PTC RESET FUSE 6V 500MA 1206</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>F2112CT-ND</t>
+  </si>
+  <si>
+    <t>Littelfuse Inc.</t>
+  </si>
+  <si>
+    <t>RES SMD 1K OHM 1% 1/8W 0603</t>
+  </si>
+  <si>
+    <t>R8, R23, R24</t>
+  </si>
+  <si>
+    <t>MCT0603-1.00K-CFCT-ND</t>
+  </si>
+  <si>
+    <t>MCT06030C1001FP500</t>
+  </si>
+  <si>
+    <t>RES SMD 10K OHM 1% 1/8W 0603</t>
+  </si>
+  <si>
+    <t>R2, R6</t>
+  </si>
+  <si>
+    <t>MCT0603-10.0K-CFCT-ND</t>
+  </si>
+  <si>
+    <t>MCT06030C1002FP500</t>
+  </si>
+  <si>
+    <t>RES SMD 2.2K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>P2.20KHCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF2201V</t>
+  </si>
+  <si>
+    <t>RES SMD 3.3K OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R5, R7, R9, R10, R13, R20, R21</t>
+  </si>
+  <si>
+    <t>P3.3KGCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-3GEYJ332V</t>
+  </si>
+  <si>
+    <t>RES SMD 100K OHM 0.1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>RG16P100KBCT-ND</t>
+  </si>
+  <si>
+    <t>RG1608P-104-B-T5</t>
   </si>
   <si>
     <t>.050" X .050 TERMINAL STRIP</t>
@@ -229,12 +439,6 @@
     <t>FTSH-105-01-F-DV-K-TR</t>
   </si>
   <si>
-    <t>Header, 10-Pin</t>
-  </si>
-  <si>
-    <t>P5</t>
-  </si>
-  <si>
     <t>.025 SQ. TERMINAL STRIPS</t>
   </si>
   <si>
@@ -245,201 +449,6 @@
   </si>
   <si>
     <t>TSM-110-01-L-DH-A-P-TR</t>
-  </si>
-  <si>
-    <t>PTC RESET FUSE 6V 500MA 1206</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>F2112CT-ND</t>
-  </si>
-  <si>
-    <t>Littelfuse Inc.</t>
-  </si>
-  <si>
-    <t>RES SMD 10K OHM 1% 1/8W 0603</t>
-  </si>
-  <si>
-    <t>R2, R6</t>
-  </si>
-  <si>
-    <t>MCT0603-10.0K-CFCT-ND</t>
-  </si>
-  <si>
-    <t>MCT06030C1002FP500</t>
-  </si>
-  <si>
-    <t>RES 0 OHM JUMPER 1/8W 0603</t>
-  </si>
-  <si>
-    <t>R3, R11, R25</t>
-  </si>
-  <si>
-    <t>749-1745-1-ND</t>
-  </si>
-  <si>
-    <t>MCT0603MZ0000ZP500</t>
-  </si>
-  <si>
-    <t>RES SMD 2.2K OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>P2.20KHCT-ND</t>
-  </si>
-  <si>
-    <t>ERJ-3EKF2201V</t>
-  </si>
-  <si>
-    <t>RES SMD 3.3K OHM 5% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>R5, R7, R9, R10, R13, R20, R21</t>
-  </si>
-  <si>
-    <t>P3.3KGCT-ND</t>
-  </si>
-  <si>
-    <t>ERJ-3GEYJ332V</t>
-  </si>
-  <si>
-    <t>RES SMD 1K OHM 1% 1/8W 0603</t>
-  </si>
-  <si>
-    <t>R8, R23, R24</t>
-  </si>
-  <si>
-    <t>MCT0603-1.00K-CFCT-ND</t>
-  </si>
-  <si>
-    <t>MCT06030C1001FP500</t>
-  </si>
-  <si>
-    <t>RES SMD 100K OHM 0.1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>RG16P100KBCT-ND</t>
-  </si>
-  <si>
-    <t>RG1608P-104-B-T5</t>
-  </si>
-  <si>
-    <t>RES SMD 1M OHM 5% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>R16, R17</t>
-  </si>
-  <si>
-    <t>1276-5134-1-ND</t>
-  </si>
-  <si>
-    <t>RC1608J105CS</t>
-  </si>
-  <si>
-    <t>RES SMD 100 OHM 5% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>R18, R19, R22</t>
-  </si>
-  <si>
-    <t>541-4059-1-ND</t>
-  </si>
-  <si>
-    <t>CRCW0603100RJNEAC</t>
-  </si>
-  <si>
-    <t>SWITCH SLIDE SPDT 100MA 12V</t>
-  </si>
-  <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t>401-2012-1-ND</t>
-  </si>
-  <si>
-    <t>AYZ0102AGRLC</t>
-  </si>
-  <si>
-    <t>MHS22204=DPDT SL SW VERT AG</t>
-  </si>
-  <si>
-    <t>S2</t>
-  </si>
-  <si>
-    <t>450-1572-ND</t>
-  </si>
-  <si>
-    <t>1825289-1</t>
-  </si>
-  <si>
-    <t>SWITCH TACTILE SPST-NO 0.05A 12V</t>
-  </si>
-  <si>
-    <t>S3, S4, S5</t>
-  </si>
-  <si>
-    <t>732-7004-1-ND</t>
-  </si>
-  <si>
-    <t>430182043816</t>
-  </si>
-  <si>
-    <t>PC TEST POINT MINIATURE</t>
-  </si>
-  <si>
-    <t>TP1, TP2, TP3, TP5, TP6, TP10, TP11</t>
-  </si>
-  <si>
-    <t>36-5019CT-ND</t>
-  </si>
-  <si>
-    <t>5019</t>
-  </si>
-  <si>
-    <t>IC LI-ION CHARGE MGMT 16-QFN</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>BQ24075RGTR</t>
-  </si>
-  <si>
-    <t>Tiny Single Inductor Buck Boost Converter 12-VQFN -40 to 85</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>296-42650-1-ND</t>
-  </si>
-  <si>
-    <t>TPS63051RMWR</t>
-  </si>
-  <si>
-    <t>EFR32BG13 Bluetooth 5.0 Module, 512kB Flash, +8dbm</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>USB Bridge, USB to UART USB 2.0 UART Interface 28-SSOP</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>768-1007-1-ND</t>
-  </si>
-  <si>
-    <t>FT232RL-REEL</t>
   </si>
 </sst>
 </file>
@@ -822,14 +831,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DA8D8A-731B-45AB-9B24-CCC041853544}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0EE5A3E-050A-4AEA-A526-845DCBCAC042}">
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="21.5703125" customWidth="1"/>
+    <col min="1" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -860,7 +872,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
@@ -868,101 +880,101 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E3" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="E4" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="E5" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E6" s="3">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E7" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E8" s="3">
         <v>1</v>
@@ -970,16 +982,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E9" s="3">
         <v>1</v>
@@ -987,16 +999,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="C10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="E10" s="3">
         <v>1</v>
@@ -1004,33 +1016,33 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="E11" s="3">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="D12" s="2" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E12" s="3">
         <v>1</v>
@@ -1038,16 +1050,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
@@ -1055,33 +1067,33 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="E14" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E15" s="3">
         <v>1</v>
@@ -1089,16 +1101,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E16" s="3">
         <v>1</v>
@@ -1106,16 +1118,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E17" s="3">
         <v>1</v>
@@ -1123,16 +1135,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E18" s="3">
         <v>1</v>
@@ -1140,33 +1152,33 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="E19" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E20" s="3">
         <v>1</v>
@@ -1174,19 +1186,19 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="E21" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1203,7 +1215,7 @@
         <v>74</v>
       </c>
       <c r="E22" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1220,7 +1232,7 @@
         <v>78</v>
       </c>
       <c r="E23" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1237,7 +1249,7 @@
         <v>82</v>
       </c>
       <c r="E24" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1254,7 +1266,7 @@
         <v>86</v>
       </c>
       <c r="E25" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1271,7 +1283,7 @@
         <v>90</v>
       </c>
       <c r="E26" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1288,7 +1300,7 @@
         <v>94</v>
       </c>
       <c r="E27" s="3">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1322,7 +1334,7 @@
         <v>102</v>
       </c>
       <c r="E29" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1339,7 +1351,7 @@
         <v>106</v>
       </c>
       <c r="E30" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1356,7 +1368,7 @@
         <v>110</v>
       </c>
       <c r="E31" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1390,7 +1402,7 @@
         <v>118</v>
       </c>
       <c r="E33" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1407,7 +1419,7 @@
         <v>122</v>
       </c>
       <c r="E34" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1424,7 +1436,7 @@
         <v>126</v>
       </c>
       <c r="E35" s="3">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1438,24 +1450,24 @@
         <v>129</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>64</v>
+        <v>130</v>
       </c>
       <c r="E36" s="3">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E37" s="3">
         <v>1</v>
@@ -1463,16 +1475,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>64</v>
+        <v>137</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>64</v>
+        <v>138</v>
       </c>
       <c r="E38" s="3">
         <v>1</v>
@@ -1480,16 +1492,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E39" s="3">
         <v>1</v>

</xml_diff>

<commit_message>
fixed BOM issues in schematic
</commit_message>
<xml_diff>
--- a/Gateway/Project Outputs for Gateway/Gateway.xlsx
+++ b/Gateway/Project Outputs for Gateway/Gateway.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CDFB0248-E50D-410E-8DFF-6D3B1AE7ABD5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9B4D373-6D56-4D1A-B2FE-CEE2567A33AA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13110" windowHeight="7995" xr2:uid="{F8D59719-2269-440C-ABEA-8661FA29D0C1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13110" windowHeight="7995" xr2:uid="{A49CE77A-EAFE-40E9-992E-C276F3E4BB46}"/>
   </bookViews>
   <sheets>
     <sheet name="Gateway" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="141">
   <si>
     <t>Description</t>
   </si>
@@ -37,6 +37,66 @@
     <t>Quantity</t>
   </si>
   <si>
+    <t>.025 SQ. TERMINAL STRIPS</t>
+  </si>
+  <si>
+    <t>P6</t>
+  </si>
+  <si>
+    <t>SAM14883CT-ND</t>
+  </si>
+  <si>
+    <t>TSM-110-01-L-DH-A-P-TR</t>
+  </si>
+  <si>
+    <t>.050" X .050 TERMINAL STRIP</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>SAM13160CT-ND</t>
+  </si>
+  <si>
+    <t>FTSH-105-01-F-DV-K-TR</t>
+  </si>
+  <si>
+    <t>Blue 470nm LED Indication - Discrete 2.85V 0603 (1608 Metric)</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>475-2816-1-ND</t>
+  </si>
+  <si>
+    <t>LB Q39G-L2OO-35-1</t>
+  </si>
+  <si>
+    <t>CONN HEADER PH SIDE 2POS 2MM SMD</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>455-1749-1-ND</t>
+  </si>
+  <si>
+    <t>S2B-PH-SM4-TB(LF)(SN)</t>
+  </si>
+  <si>
+    <t>EFR32BG13 Bluetooth 5.0 Module, 512kB Flash, +8dbm</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>336-5465-1-ND</t>
+  </si>
+  <si>
+    <t>BGM13P22F512GA-V2</t>
+  </si>
+  <si>
     <t>Header, 10-Pin</t>
   </si>
   <si>
@@ -52,6 +112,87 @@
     <t>P2, P3</t>
   </si>
   <si>
+    <t>IC LI-ION CHARGE MGMT 16-QFN</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>296-38874-1-ND</t>
+  </si>
+  <si>
+    <t>BQ24075RGTT</t>
+  </si>
+  <si>
+    <t>LED GREEN DIFFUSED 0603 SMD</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>475-3118-1-ND</t>
+  </si>
+  <si>
+    <t>LG L29K-F2J1-24-Z</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>LED RED DIFFUSED 0603 SMD</t>
+  </si>
+  <si>
+    <t>D23</t>
+  </si>
+  <si>
+    <t>475-1195-1-ND</t>
+  </si>
+  <si>
+    <t>LS L29K-H1J2-1-Z</t>
+  </si>
+  <si>
+    <t>LED YELLOW DIFFUSED 0603 SMD</t>
+  </si>
+  <si>
+    <t>D24</t>
+  </si>
+  <si>
+    <t>475-1196-1-ND</t>
+  </si>
+  <si>
+    <t>LY L29K-H1K2-26-Z</t>
+  </si>
+  <si>
+    <t>MHS22204=DPDT SL SW VERT AG</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>450-1572-ND</t>
+  </si>
+  <si>
+    <t>1825289-1</t>
+  </si>
+  <si>
+    <t>Micro Usb, 2.0 Type Ab, Receptacle, Th</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>609-4053-1-ND</t>
+  </si>
+  <si>
+    <t>10104111-0001LF</t>
+  </si>
+  <si>
     <t>PC TEST POINT MINIATURE</t>
   </si>
   <si>
@@ -64,10 +205,58 @@
     <t>5019</t>
   </si>
   <si>
+    <t>PTC RESET FUSE 6V 500MA 1206</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>F2112CT-ND</t>
+  </si>
+  <si>
+    <t>Littelfuse Inc.</t>
+  </si>
+  <si>
+    <t>SWITCH SLIDE SPDT 100MA 12V</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>401-2012-1-ND</t>
+  </si>
+  <si>
+    <t>AYZ0102AGRLC</t>
+  </si>
+  <si>
+    <t>SWITCH TACTILE SPST-NO 0.05A 12V</t>
+  </si>
+  <si>
+    <t>S3, S4, S5</t>
+  </si>
+  <si>
+    <t>732-7004-1-ND</t>
+  </si>
+  <si>
+    <t>430182043816</t>
+  </si>
+  <si>
+    <t>Tiny Single Inductor Buck Boost Converter 12-VQFN -40 to 85</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>296-42650-1-ND</t>
+  </si>
+  <si>
+    <t>TPS63051RMWR</t>
+  </si>
+  <si>
     <t>TVS DIODE 5.5V 14V 2X1SON</t>
   </si>
   <si>
-    <t>D18, D19, D20, D21, D22</t>
+    <t>D4, D8, D9, D10, D11, D12, D13, D14, D15, D16, D17, D18, D19, D20, D21, D22, D25, D26, D27, D28, D29</t>
   </si>
   <si>
     <t>296-30406-1-ND</t>
@@ -76,46 +265,76 @@
     <t>TPD1E10B06DPYR</t>
   </si>
   <si>
-    <t>Zener Diode</t>
-  </si>
-  <si>
-    <t>D4, D8, D9, D10, D11, D12, D13, D14, D15, D16, D17, D25, D26, D27, D28, D29</t>
-  </si>
-  <si>
-    <t>IC LI-ION CHARGE MGMT 16-QFN</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>296-38874-1-ND</t>
-  </si>
-  <si>
-    <t>BQ24075RGTR</t>
-  </si>
-  <si>
-    <t>Tiny Single Inductor Buck Boost Converter 12-VQFN -40 to 85</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>296-42650-1-ND</t>
-  </si>
-  <si>
-    <t>TPS63051RMWR</t>
-  </si>
-  <si>
-    <t>EFR32BG13 Bluetooth 5.0 Module, 512kB Flash, +8dbm</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>336-5465-1-ND</t>
-  </si>
-  <si>
-    <t>BGM13P22F512GA-V2</t>
+    <t>USB Bridge, USB to UART USB 2.0 UART Interface 28-SSOP</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>768-1007-1-ND</t>
+  </si>
+  <si>
+    <t>FT232RL-REEL</t>
+  </si>
+  <si>
+    <t>RES 0 OHM JUMPER 1/8W 0603</t>
+  </si>
+  <si>
+    <t>R3, R11, R25, R26</t>
+  </si>
+  <si>
+    <t>749-1745-1-ND</t>
+  </si>
+  <si>
+    <t>MCT0603MZ0000ZP500</t>
+  </si>
+  <si>
+    <t>RES SMD 1K OHM 1% 1/8W 0603</t>
+  </si>
+  <si>
+    <t>R8, R23, R24</t>
+  </si>
+  <si>
+    <t>MCT0603-1.00K-CFCT-ND</t>
+  </si>
+  <si>
+    <t>MCT06030C1001FP500</t>
+  </si>
+  <si>
+    <t>RES SMD 1M OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R16, R17</t>
+  </si>
+  <si>
+    <t>1276-5134-1-ND</t>
+  </si>
+  <si>
+    <t>RC1608J105CS</t>
+  </si>
+  <si>
+    <t>CAP CER 1000PF 50V X7R 0603</t>
+  </si>
+  <si>
+    <t>C9, C10</t>
+  </si>
+  <si>
+    <t>478-5006-1-ND</t>
+  </si>
+  <si>
+    <t>06035C102JAT2A</t>
+  </si>
+  <si>
+    <t>CAP CER 1UF 10V X7R 0603</t>
+  </si>
+  <si>
+    <t>C1, C3, C7</t>
+  </si>
+  <si>
+    <t>1276-1946-1-ND</t>
+  </si>
+  <si>
+    <t>CL10B105KP8NNNC</t>
   </si>
   <si>
     <t>CAP CER 1300PF 25V C0G/NP0 0603</t>
@@ -130,109 +349,76 @@
     <t>C0603C132J3GAC7867</t>
   </si>
   <si>
-    <t>SWITCH SLIDE SPDT 100MA 12V</t>
-  </si>
-  <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t>401-2012-1-ND</t>
-  </si>
-  <si>
-    <t>AYZ0102AGRLC</t>
-  </si>
-  <si>
-    <t>MHS22204=DPDT SL SW VERT AG</t>
-  </si>
-  <si>
-    <t>S2</t>
-  </si>
-  <si>
-    <t>450-1572-ND</t>
-  </si>
-  <si>
-    <t>1825289-1</t>
-  </si>
-  <si>
-    <t>CONN HEADER PH SIDE 2POS 2MM SMD</t>
-  </si>
-  <si>
-    <t>B1</t>
-  </si>
-  <si>
-    <t>455-1749-1-ND</t>
-  </si>
-  <si>
-    <t>S2B-PH-SM4-TB(LF)(SN)</t>
-  </si>
-  <si>
-    <t>LED RED DIFFUSED 0603 SMD</t>
-  </si>
-  <si>
-    <t>D23</t>
-  </si>
-  <si>
-    <t>475-1195-1-ND</t>
-  </si>
-  <si>
-    <t>LS L29K-H1J2-1-Z</t>
-  </si>
-  <si>
-    <t>LED YELLOW DIFFUSED 0603 SMD</t>
-  </si>
-  <si>
-    <t>D24</t>
-  </si>
-  <si>
-    <t>475-1196-1-ND</t>
-  </si>
-  <si>
-    <t>LY L29K-H1K2-26-Z</t>
-  </si>
-  <si>
-    <t>Blue 470nm LED Indication - Discrete 2.85V 0603 (1608 Metric)</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>475-2816-1-ND</t>
-  </si>
-  <si>
-    <t>LB Q39G-L2OO-35-1</t>
-  </si>
-  <si>
-    <t>LED GREEN DIFFUSED 0603 SMD</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>475-3118-1-ND</t>
-  </si>
-  <si>
-    <t>LG L29K-F2J1-24-Z</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>D6</t>
-  </si>
-  <si>
-    <t>D7</t>
-  </si>
-  <si>
-    <t>CAP CER 1000PF 50V X7R 0603</t>
-  </si>
-  <si>
-    <t>C9, C10</t>
-  </si>
-  <si>
-    <t>478-5006-1-ND</t>
-  </si>
-  <si>
-    <t>06035C102JAT2A</t>
+    <t>FIXED IND 1.5UH 1.1A 213 MOHM</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>490-15637-1-ND</t>
+  </si>
+  <si>
+    <t>LQM18PN1R5MFHD</t>
+  </si>
+  <si>
+    <t>RES SMD 2.2K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>P2.20KHCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF2201V</t>
+  </si>
+  <si>
+    <t>RES SMD 3.3K OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R5, R7, R9, R10, R13, R20, R21</t>
+  </si>
+  <si>
+    <t>P3.3KGCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-3GEYJ332V</t>
+  </si>
+  <si>
+    <t>RES SMD 10K OHM 1% 1/8W 0603</t>
+  </si>
+  <si>
+    <t>R2, R6</t>
+  </si>
+  <si>
+    <t>MCT0603-10.0K-CFCT-ND</t>
+  </si>
+  <si>
+    <t>MCT06030C1002FP500</t>
+  </si>
+  <si>
+    <t>CAP CER 22UF 10V X5R 0603</t>
+  </si>
+  <si>
+    <t>C2, C4, C6, C8, C13</t>
+  </si>
+  <si>
+    <t>1276-6504-1-ND</t>
+  </si>
+  <si>
+    <t>CL10A226MPCNUBE</t>
+  </si>
+  <si>
+    <t>RES SMD 100K OHM 0.1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>RG16P100KBCT-ND</t>
+  </si>
+  <si>
+    <t>RG1608P-104-B-T5</t>
   </si>
   <si>
     <t>CAP CER 0.1UF 16V X7R 0603</t>
@@ -247,42 +433,6 @@
     <t>0603YC104MAT4A</t>
   </si>
   <si>
-    <t>CAP CER 0.1UF 25V X7R 0603</t>
-  </si>
-  <si>
-    <t>C1, C3, C7</t>
-  </si>
-  <si>
-    <t>490-6051-1-ND</t>
-  </si>
-  <si>
-    <t>GCM188R71E104KA57D</t>
-  </si>
-  <si>
-    <t>CAP CER 10UF 10V X5R 0603</t>
-  </si>
-  <si>
-    <t>C2, C4, C6, C8, C13</t>
-  </si>
-  <si>
-    <t>490-10474-1-ND</t>
-  </si>
-  <si>
-    <t>GRM188R61A106KE69D</t>
-  </si>
-  <si>
-    <t>FIXED IND 1.5UH 1.1A 213 MOHM</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>490-15637-1-ND</t>
-  </si>
-  <si>
-    <t>LQM18PN1R5MFHD</t>
-  </si>
-  <si>
     <t>RES SMD 100 OHM 5% 1/10W 0603</t>
   </si>
   <si>
@@ -293,162 +443,6 @@
   </si>
   <si>
     <t>CRCW0603100RJNEAC</t>
-  </si>
-  <si>
-    <t>Micro Usb, 2.0 Type Ab, Receptacle, Th</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>609-4053-1-ND</t>
-  </si>
-  <si>
-    <t>10104111-0001LF</t>
-  </si>
-  <si>
-    <t>SWITCH TACTILE SPST-NO 0.05A 12V</t>
-  </si>
-  <si>
-    <t>S3, S4, S5</t>
-  </si>
-  <si>
-    <t>732-7004-1-ND</t>
-  </si>
-  <si>
-    <t>430182043816</t>
-  </si>
-  <si>
-    <t>RES 0 OHM JUMPER 1/8W 0603</t>
-  </si>
-  <si>
-    <t>R3, R11, R25</t>
-  </si>
-  <si>
-    <t>749-1745-1-ND</t>
-  </si>
-  <si>
-    <t>MCT0603MZ0000ZP500</t>
-  </si>
-  <si>
-    <t>USB Bridge, USB to UART USB 2.0 UART Interface 28-SSOP</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>768-1007-1-ND</t>
-  </si>
-  <si>
-    <t>FT232RL-REEL</t>
-  </si>
-  <si>
-    <t>RES SMD 1M OHM 5% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>R16, R17</t>
-  </si>
-  <si>
-    <t>1276-5134-1-ND</t>
-  </si>
-  <si>
-    <t>RC1608J105CS</t>
-  </si>
-  <si>
-    <t>PTC RESET FUSE 6V 500MA 1206</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>F2112CT-ND</t>
-  </si>
-  <si>
-    <t>Littelfuse Inc.</t>
-  </si>
-  <si>
-    <t>RES SMD 1K OHM 1% 1/8W 0603</t>
-  </si>
-  <si>
-    <t>R8, R23, R24</t>
-  </si>
-  <si>
-    <t>MCT0603-1.00K-CFCT-ND</t>
-  </si>
-  <si>
-    <t>MCT06030C1001FP500</t>
-  </si>
-  <si>
-    <t>RES SMD 10K OHM 1% 1/8W 0603</t>
-  </si>
-  <si>
-    <t>R2, R6</t>
-  </si>
-  <si>
-    <t>MCT0603-10.0K-CFCT-ND</t>
-  </si>
-  <si>
-    <t>MCT06030C1002FP500</t>
-  </si>
-  <si>
-    <t>RES SMD 2.2K OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>P2.20KHCT-ND</t>
-  </si>
-  <si>
-    <t>ERJ-3EKF2201V</t>
-  </si>
-  <si>
-    <t>RES SMD 3.3K OHM 5% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>R5, R7, R9, R10, R13, R20, R21</t>
-  </si>
-  <si>
-    <t>P3.3KGCT-ND</t>
-  </si>
-  <si>
-    <t>ERJ-3GEYJ332V</t>
-  </si>
-  <si>
-    <t>RES SMD 100K OHM 0.1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>RG16P100KBCT-ND</t>
-  </si>
-  <si>
-    <t>RG1608P-104-B-T5</t>
-  </si>
-  <si>
-    <t>.050" X .050 TERMINAL STRIP</t>
-  </si>
-  <si>
-    <t>P4</t>
-  </si>
-  <si>
-    <t>SAM13160CT-ND</t>
-  </si>
-  <si>
-    <t>FTSH-105-01-F-DV-K-TR</t>
-  </si>
-  <si>
-    <t>.025 SQ. TERMINAL STRIPS</t>
-  </si>
-  <si>
-    <t>P6</t>
-  </si>
-  <si>
-    <t>SAM14883CT-ND</t>
-  </si>
-  <si>
-    <t>TSM-110-01-L-DH-A-P-TR</t>
   </si>
 </sst>
 </file>
@@ -831,8 +825,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0EE5A3E-050A-4AEA-A526-845DCBCAC042}">
-  <dimension ref="A1:E39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62C9C96B-2775-4773-A497-E565128FD91F}">
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -872,7 +866,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
@@ -880,84 +874,84 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E3" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E4" s="3">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E5" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E6" s="3">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
@@ -965,33 +959,33 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E8" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E9" s="3">
         <v>1</v>
@@ -999,16 +993,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E10" s="3">
         <v>1</v>
@@ -1016,16 +1010,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="E11" s="3">
         <v>1</v>
@@ -1033,16 +1027,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E12" s="3">
         <v>1</v>
@@ -1050,16 +1044,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
@@ -1067,16 +1061,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E14" s="3">
         <v>1</v>
@@ -1084,16 +1078,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E15" s="3">
         <v>1</v>
@@ -1101,16 +1095,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E16" s="3">
         <v>1</v>
@@ -1118,16 +1112,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E17" s="3">
         <v>1</v>
@@ -1135,33 +1129,33 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="E18" s="3">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E19" s="3">
         <v>1</v>
@@ -1169,16 +1163,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="E20" s="3">
         <v>1</v>
@@ -1186,101 +1180,101 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E21" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E22" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E23" s="3">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E24" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E25" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E26" s="3">
         <v>3</v>
@@ -1288,50 +1282,50 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E27" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E28" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E29" s="3">
         <v>3</v>
@@ -1339,16 +1333,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E30" s="3">
         <v>1</v>
@@ -1356,33 +1350,33 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E31" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E32" s="3">
         <v>1</v>
@@ -1390,33 +1384,33 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E33" s="3">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E34" s="3">
         <v>2</v>
@@ -1424,87 +1418,70 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E35" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E36" s="3">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E37" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E38" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E39" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>